<commit_message>
Update Subject data T2DM iHMP 2.xlsx
</commit_message>
<xml_diff>
--- a/T2DM iHMP Data/subject data/Subject data T2DM iHMP 2.xlsx
+++ b/T2DM iHMP Data/subject data/Subject data T2DM iHMP 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\T2DM iHMP Data\subject data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\T2DM iHMP Data\subject data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55773726-7673-4AF1-A1EF-802B30261711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18073554-0522-4FFA-906C-4A45FB15C3ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9020" yWindow="0" windowWidth="10220" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10490" yWindow="0" windowWidth="8720" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -644,9 +644,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -681,6 +678,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1730,35 +1730,35 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="30" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="31" t="s">
+    <row r="27" spans="1:10" s="29" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="31" t="s">
+      <c r="B27" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="31">
+      <c r="D27" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="30">
         <v>59.12</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="30">
         <v>25.91</v>
       </c>
-      <c r="G27" s="31">
+      <c r="G27" s="30">
         <v>111</v>
       </c>
-      <c r="H27" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="33">
+      <c r="H27" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="32">
         <v>15</v>
       </c>
-      <c r="J27" s="30" t="s">
+      <c r="J27" s="29" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1849,35 +1849,35 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="30" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="27" t="s">
+    <row r="31" spans="1:10" s="29" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="27">
+      <c r="B31" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="26">
         <v>48.86</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="26">
         <v>37.42</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="26">
         <v>257</v>
       </c>
-      <c r="H31" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="29">
+      <c r="H31" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="28">
         <v>13</v>
       </c>
-      <c r="J31" s="30" t="s">
+      <c r="J31" s="29" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1910,35 +1910,35 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="30" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="27" t="s">
+    <row r="33" spans="1:10" s="29" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="27">
+      <c r="B33" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="26">
         <v>55.92</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="26">
         <v>27.34</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="26">
         <v>166</v>
       </c>
-      <c r="H33" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="29">
-        <v>14</v>
-      </c>
-      <c r="J33" s="30" t="s">
+      <c r="H33" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="28">
+        <v>14</v>
+      </c>
+      <c r="J33" s="29" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2058,35 +2058,35 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="30" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="31" t="s">
+    <row r="38" spans="1:10" s="29" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="31">
+      <c r="B38" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="30">
         <v>47.19</v>
       </c>
-      <c r="F38" s="31">
+      <c r="F38" s="30">
         <v>30.33</v>
       </c>
-      <c r="G38" s="31">
+      <c r="G38" s="30">
         <v>71</v>
       </c>
-      <c r="H38" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="33">
+      <c r="H38" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="32">
         <v>20</v>
       </c>
-      <c r="J38" s="30" t="s">
+      <c r="J38" s="29" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2119,67 +2119,67 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="34" t="s">
+    <row r="40" spans="1:10" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="34">
+      <c r="B40" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="33">
         <v>45.06</v>
       </c>
-      <c r="F40" s="34">
+      <c r="F40" s="33">
         <v>24.89</v>
       </c>
-      <c r="G40" s="34">
+      <c r="G40" s="33">
         <v>61</v>
       </c>
-      <c r="H40" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="I40" s="36">
+      <c r="H40" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="35">
         <v>22</v>
       </c>
-      <c r="J40" s="30" t="s">
+      <c r="J40" s="29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="26" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="22" t="s">
+    <row r="41" spans="1:10" s="25" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="23">
+      <c r="B41" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="22">
         <v>61.94</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="22">
         <v>29.47</v>
       </c>
-      <c r="G41" s="23">
+      <c r="G41" s="22">
         <v>224.6</v>
       </c>
-      <c r="H41" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="I41" s="25">
-        <v>18</v>
-      </c>
-      <c r="J41" s="26" t="s">
+      <c r="H41" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="24">
+        <v>18</v>
+      </c>
+      <c r="J41" s="25" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>